<commit_message>
last fix at style.css
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maor\Desktop\semeter f\סביבות\3.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maor\Desktop\VancouverWeb-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964993CB-3FDC-4695-A9F4-F85EFA29BFC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12811A1D-7230-4258-86DD-49A349756B1E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5EAC4555-576B-4BCB-BEA8-34FF6D2B9292}"/>
   </bookViews>
@@ -271,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,11 +299,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -580,9 +575,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -604,7 +596,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -613,6 +604,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007EAF-2B8B-4A80-98FD-1B19E698AA25}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,7 +975,7 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="29" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1001,7 +998,7 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>51</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1041,13 +1038,13 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="8"/>
@@ -1062,13 +1059,13 @@
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -1308,48 +1305,48 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="23">
+      <c r="A17" s="22">
         <v>16</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="25" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="27">
+      <c r="A18" s="30">
         <v>17</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="27" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>